<commit_message>
Adjust analyzer paramters and code.
Change-Id: I54db083b378938809294e8619081e9e9fb11d81d
</commit_message>
<xml_diff>
--- a/Doc/FinanceAnalysisAlgorithm.xlsx
+++ b/Doc/FinanceAnalysisAlgorithm.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5252B0-E476-4531-B66A-67FDB10F2FD7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D244E5-5CB5-402D-A93D-A0FBBEEA87F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="财务分析" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="67">
   <si>
     <t>存贷双高</t>
   </si>
@@ -95,18 +95,6 @@
     <t>非主营业务占比过高</t>
   </si>
   <si>
-    <t>营业收入，主营业务收入，其他业务收入</t>
-  </si>
-  <si>
-    <t>主营业务收入 = 营业收入 - 其他业务收入</t>
-  </si>
-  <si>
-    <t>TuShare中没有主营业务收入数据</t>
-  </si>
-  <si>
-    <t>【主营业务收入】/【营业收入】 &gt; 50%</t>
-  </si>
-  <si>
     <t>50%为不可靠经验值</t>
   </si>
   <si>
@@ -194,9 +182,6 @@
     <t>商誉过高</t>
   </si>
   <si>
-    <t>商誉，资产总计，净资产</t>
-  </si>
-  <si>
     <t>商誉占总资产比例 = 商誉 / 资产总计</t>
   </si>
   <si>
@@ -219,6 +204,24 @@
   </si>
   <si>
     <t>从财务费用及利息收入的角度分析：支付的利息高，而现金带来的利息收益极低</t>
+  </si>
+  <si>
+    <t>e6ab71a9-0c9f-4500-b2db-d682af567f70</t>
+  </si>
+  <si>
+    <t>商誉，资产总计，负债合计</t>
+  </si>
+  <si>
+    <t>净资产 = 资产总计 - 负债合计</t>
+  </si>
+  <si>
+    <t>营业收入，其他业务收入</t>
+  </si>
+  <si>
+    <t>其它业务收入占比 = 其他业务收入 / 营业收入</t>
+  </si>
+  <si>
+    <t>【其它业务收入占比】 &gt; 50%</t>
   </si>
 </sst>
 </file>
@@ -806,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E138"/>
+  <dimension ref="B1:E139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,17 +846,17 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E5" s="16"/>
     </row>
@@ -863,7 +866,7 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E6" s="8"/>
     </row>
@@ -881,7 +884,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E8" s="8"/>
     </row>
@@ -897,7 +900,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E10" s="8"/>
     </row>
@@ -913,7 +916,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E12" s="8"/>
     </row>
@@ -929,7 +932,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E14" s="8"/>
     </row>
@@ -945,7 +948,7 @@
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E16" s="11"/>
     </row>
@@ -956,17 +959,17 @@
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E20" s="16"/>
     </row>
@@ -976,7 +979,7 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E21" s="8"/>
     </row>
@@ -994,7 +997,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E23" s="8"/>
     </row>
@@ -1010,7 +1013,7 @@
         <v>9</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E25" s="8"/>
     </row>
@@ -1032,7 +1035,7 @@
         <v>17</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E28" s="8"/>
     </row>
@@ -1048,7 +1051,7 @@
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E30" s="8"/>
     </row>
@@ -1064,7 +1067,7 @@
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E32" s="11"/>
     </row>
@@ -1081,11 +1084,11 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E36" s="8"/>
     </row>
@@ -1095,7 +1098,7 @@
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E37" s="8"/>
     </row>
@@ -1113,11 +1116,9 @@
         <v>8</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>26</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E39" s="8"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="7"/>
@@ -1139,10 +1140,10 @@
       <c r="B42" s="7"/>
       <c r="C42" s="2"/>
       <c r="D42" s="12" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.3">
@@ -1157,7 +1158,7 @@
         <v>17</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E44" s="8"/>
     </row>
@@ -1173,7 +1174,7 @@
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E46" s="8"/>
     </row>
@@ -1189,7 +1190,7 @@
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E48" s="11"/>
     </row>
@@ -1212,11 +1213,11 @@
     </row>
     <row r="52" spans="2:5" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B52" s="25" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E52" s="26"/>
     </row>
@@ -1334,7 +1335,7 @@
       <c r="B66" s="7"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E66" s="8"/>
     </row>
@@ -1342,7 +1343,7 @@
       <c r="B67" s="7"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E67" s="8"/>
     </row>
@@ -1358,7 +1359,7 @@
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E69" s="11"/>
     </row>
@@ -1369,17 +1370,17 @@
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E72" s="6"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" s="14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E73" s="16"/>
     </row>
@@ -1389,7 +1390,7 @@
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E74" s="8"/>
     </row>
@@ -1407,7 +1408,7 @@
         <v>8</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E76" s="8"/>
     </row>
@@ -1431,10 +1432,10 @@
       <c r="B79" s="7"/>
       <c r="C79" s="2"/>
       <c r="D79" s="12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.3">
@@ -1449,7 +1450,7 @@
         <v>17</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E81" s="8"/>
     </row>
@@ -1465,7 +1466,7 @@
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E83" s="8"/>
     </row>
@@ -1473,7 +1474,7 @@
       <c r="B84" s="7"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E84" s="8"/>
     </row>
@@ -1481,7 +1482,7 @@
       <c r="B85" s="7"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E85" s="8"/>
     </row>
@@ -1497,7 +1498,7 @@
       </c>
       <c r="C87" s="10"/>
       <c r="D87" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E87" s="11"/>
     </row>
@@ -1508,16 +1509,18 @@
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E90" s="6"/>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B91" s="14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C91" s="15"/>
-      <c r="D91" s="17"/>
+      <c r="D91" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="E91" s="16"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.3">
@@ -1526,7 +1529,7 @@
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E92" s="8"/>
     </row>
@@ -1544,7 +1547,7 @@
         <v>8</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E94" s="8"/>
     </row>
@@ -1552,31 +1555,31 @@
       <c r="B95" s="7"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E95" s="8"/>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B96" s="7"/>
       <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
+      <c r="D96" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="E96" s="8"/>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B97" s="7"/>
-      <c r="C97" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
       <c r="E97" s="8"/>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B98" s="7"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="12" t="s">
-        <v>61</v>
+      <c r="C98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="E98" s="8"/>
     </row>
@@ -1584,291 +1587,299 @@
       <c r="B99" s="7"/>
       <c r="C99" s="2"/>
       <c r="D99" s="12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E99" s="8"/>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B100" s="7"/>
       <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
+      <c r="D100" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="E100" s="8"/>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B101" s="7"/>
-      <c r="C101" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
       <c r="E101" s="8"/>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B102" s="7"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
+      <c r="C102" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="E102" s="8"/>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B103" s="7" t="s">
+      <c r="B103" s="7"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="8"/>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B104" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E103" s="8"/>
-    </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B104" s="7"/>
       <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
+      <c r="D104" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E104" s="8"/>
     </row>
-    <row r="105" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B105" s="9" t="s">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B105" s="7"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="8"/>
+    </row>
+    <row r="106" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B106" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C105" s="10"/>
-      <c r="D105" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E105" s="11"/>
-    </row>
-    <row r="107" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B108" s="4" t="s">
+      <c r="C106" s="10"/>
+      <c r="D106" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E106" s="11"/>
+    </row>
+    <row r="108" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B109" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C108" s="5"/>
-      <c r="D108" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E108" s="6"/>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B109" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C109" s="15"/>
-      <c r="D109" s="17"/>
-      <c r="E109" s="16"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E109" s="6"/>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B110" s="7" t="s">
+      <c r="B110" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C110" s="15"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="16"/>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B111" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C110" s="2"/>
-      <c r="D110" s="2"/>
-      <c r="E110" s="8"/>
-    </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B111" s="7"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
       <c r="E111" s="8"/>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B112" s="7" t="s">
+      <c r="B112" s="7"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="8"/>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B113" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E112" s="8"/>
-    </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B113" s="7"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2"/>
+      <c r="D113" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E113" s="8"/>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B114" s="7"/>
-      <c r="C114" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D114" s="12"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
       <c r="E114" s="8"/>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B115" s="7"/>
-      <c r="C115" s="2"/>
+      <c r="C115" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D115" s="12"/>
       <c r="E115" s="8"/>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B116" s="7"/>
       <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
+      <c r="D116" s="12"/>
       <c r="E116" s="8"/>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B117" s="7"/>
-      <c r="C117" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
       <c r="E117" s="8"/>
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B118" s="7"/>
-      <c r="C118" s="2"/>
-      <c r="D118" s="2"/>
+      <c r="C118" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="E118" s="8"/>
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B119" s="7" t="s">
+      <c r="B119" s="7"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="8"/>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B120" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E119" s="8"/>
-    </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B120" s="7"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E120" s="8"/>
     </row>
     <row r="121" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B121" s="7"/>
       <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
+      <c r="D121" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E121" s="8"/>
     </row>
-    <row r="122" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B122" s="9" t="s">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B122" s="7"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="8"/>
+    </row>
+    <row r="123" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B123" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C122" s="10"/>
-      <c r="D122" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E122" s="11"/>
-    </row>
-    <row r="124" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B125" s="4" t="s">
+      <c r="C123" s="10"/>
+      <c r="D123" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E123" s="11"/>
+    </row>
+    <row r="125" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B126" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C125" s="5"/>
-      <c r="D125" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E125" s="6"/>
-    </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B126" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C126" s="15"/>
-      <c r="D126" s="17"/>
-      <c r="E126" s="16"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E126" s="6"/>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B127" s="7" t="s">
+      <c r="B127" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C127" s="15"/>
+      <c r="D127" s="17"/>
+      <c r="E127" s="16"/>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B128" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="8"/>
-    </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B128" s="7"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
       <c r="E128" s="8"/>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B129" s="7" t="s">
+      <c r="B129" s="7"/>
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="8"/>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B130" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C130" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D129" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E129" s="8"/>
-    </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B130" s="7"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="2"/>
+      <c r="D130" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E130" s="8"/>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B131" s="7"/>
-      <c r="C131" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D131" s="12"/>
+      <c r="C131" s="2"/>
+      <c r="D131" s="2"/>
       <c r="E131" s="8"/>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B132" s="7"/>
-      <c r="C132" s="2"/>
+      <c r="C132" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D132" s="12"/>
       <c r="E132" s="8"/>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B133" s="7"/>
       <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
+      <c r="D133" s="12"/>
       <c r="E133" s="8"/>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B134" s="7"/>
-      <c r="C134" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="C134" s="2"/>
+      <c r="D134" s="2"/>
       <c r="E134" s="8"/>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B135" s="7"/>
-      <c r="C135" s="2"/>
-      <c r="D135" s="2"/>
+      <c r="C135" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="E135" s="8"/>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B136" s="7" t="s">
+      <c r="B136" s="7"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="2"/>
+      <c r="E136" s="8"/>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B137" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C136" s="2"/>
-      <c r="D136" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E136" s="8"/>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B137" s="7"/>
       <c r="C137" s="2"/>
-      <c r="D137" s="2"/>
+      <c r="D137" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="E137" s="8"/>
     </row>
-    <row r="138" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B138" s="9" t="s">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B138" s="7"/>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="8"/>
+    </row>
+    <row r="139" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B139" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C138" s="10"/>
-      <c r="D138" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E138" s="11"/>
+      <c r="C139" s="10"/>
+      <c r="D139" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E139" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1902,7 +1913,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="17"/>
@@ -1930,7 +1941,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E7" s="8"/>
     </row>
@@ -1966,7 +1977,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E12" s="8"/>
     </row>
@@ -1982,7 +1993,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E14" s="8"/>
     </row>
@@ -1998,7 +2009,7 @@
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E16" s="11"/>
     </row>

</xml_diff>